<commit_message>
activiteit en aanwezigheid document en document van eisen en wensen aangepast
</commit_message>
<xml_diff>
--- a/documentatie/Activiteiten en Aanwezigheid.xlsx
+++ b/documentatie/Activiteiten en Aanwezigheid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\school\eindopdracht-stagesysteem\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56960157-3A03-48EB-BE41-B0313347CD56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A75BB18-FEE0-4969-BD4E-9D8421110704}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{FFD2E398-21D8-42EB-989A-CB0C9E410701}"/>
   </bookViews>
@@ -32,45 +32,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
-  <si>
-    <t>Naam(en)</t>
-  </si>
-  <si>
-    <t>activiteit</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
   <si>
     <t>datum</t>
   </si>
   <si>
-    <t>nicolay, gaia, izabella, marvin, christiaan</t>
-  </si>
-  <si>
-    <t>Plan van aanpak</t>
-  </si>
-  <si>
     <t>nicolay</t>
   </si>
   <si>
     <t>gaia</t>
   </si>
   <si>
-    <t>git instructies schrijven, discord server aangemaakt, gitbucket aangemaakt.</t>
-  </si>
-  <si>
-    <t>trello board aangemaakt</t>
-  </si>
-  <si>
     <t>christiaan</t>
-  </si>
-  <si>
-    <t>globaal gekeken naar wat voor data er moet komen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marvin </t>
-  </si>
-  <si>
-    <t>voorbereiden van vragen voor stakeholders</t>
   </si>
   <si>
     <t>izabella</t>
@@ -162,10 +135,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="justify" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="justify" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -480,124 +468,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDB3EC2-E9B9-4CD7-8411-EB7A03133CDF}">
-  <dimension ref="C3:F16"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="22.3984375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="141.86328125" style="4" customWidth="1"/>
     <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="163.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="242.1328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="58.06640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C3" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="6">
+        <v>43787</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="6">
+        <v>43788</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
+    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="6">
+        <v>43789</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A5" s="6">
+        <v>43790</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="6">
+        <v>43791</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C12" s="2">
-        <v>43787</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C13" s="2">
-        <v>43788</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C14" s="2">
-        <v>43789</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C15" s="2">
-        <v>43790</v>
-      </c>
-      <c r="D15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C16" s="2">
-        <v>43791</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -620,7 +568,7 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2">
         <v>43787</v>
@@ -640,120 +588,120 @@
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2">
         <v>43794</v>
@@ -773,42 +721,42 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C21" s="2">
         <v>43801</v>
@@ -828,37 +776,37 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>